<commit_message>
Ädded updated scripts in InstantOpen
</commit_message>
<xml_diff>
--- a/InstantOpen/target/classes/com/Resources/TestData.xlsx
+++ b/InstantOpen/target/classes/com/Resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v4\TDECUProjects\InstantOpen\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777F3A6F-0084-4A4A-BDA1-E6D854A0665E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB99F45-4EFC-4657-8BE4-2AD62C96AAB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2529" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2621" uniqueCount="539">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1326,9 +1326,6 @@
     <t>35688741</t>
   </si>
   <si>
-    <t>42355698</t>
-  </si>
-  <si>
     <t>65211025</t>
   </si>
   <si>
@@ -1638,7 +1635,19 @@
     <t>C23865_VerifySaveContinueOnSaveProgressPage</t>
   </si>
   <si>
-    <t>66875678</t>
+    <t>C23906_VerifyFundTransferWithElectronicCheck</t>
+  </si>
+  <si>
+    <t>C23907_VerifyFundTransferWithDebitCard</t>
+  </si>
+  <si>
+    <t>C23908_VerifyFundTransferOptions</t>
+  </si>
+  <si>
+    <t>C23909_VerifyApplicationSubmittion</t>
+  </si>
+  <si>
+    <t>42355451</t>
   </si>
 </sst>
 </file>
@@ -2030,10 +2039,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F129"/>
+  <dimension ref="A1:F133"/>
   <sheetViews>
-    <sheetView topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="A127" sqref="A127:XFD129"/>
+    <sheetView topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3363,7 +3372,7 @@
     </row>
     <row r="87" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>8</v>
@@ -3457,7 +3466,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>8</v>
@@ -3472,7 +3481,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>8</v>
@@ -3487,7 +3496,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>8</v>
@@ -3502,7 +3511,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>8</v>
@@ -3517,7 +3526,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>8</v>
@@ -3532,7 +3541,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>8</v>
@@ -3547,7 +3556,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>8</v>
@@ -3561,7 +3570,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B100" s="4" t="s">
         <v>8</v>
@@ -3575,7 +3584,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>8</v>
@@ -3589,7 +3598,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>8</v>
@@ -3603,7 +3612,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>8</v>
@@ -3617,7 +3626,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B104" s="4" t="s">
         <v>8</v>
@@ -3631,7 +3640,7 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>8</v>
@@ -3645,7 +3654,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>8</v>
@@ -3659,7 +3668,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B107" s="4" t="s">
         <v>8</v>
@@ -3673,7 +3682,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>8</v>
@@ -3687,7 +3696,7 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B109" s="4" t="s">
         <v>8</v>
@@ -3701,7 +3710,7 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B110" s="4" t="s">
         <v>8</v>
@@ -3715,7 +3724,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B111" s="4" t="s">
         <v>8</v>
@@ -3729,7 +3738,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B112" s="4" t="s">
         <v>8</v>
@@ -3743,7 +3752,7 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B113" s="4" t="s">
         <v>8</v>
@@ -3757,7 +3766,7 @@
     </row>
     <row r="114" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B114" s="4" t="s">
         <v>8</v>
@@ -3773,7 +3782,7 @@
     </row>
     <row r="115" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B115" s="4" t="s">
         <v>8</v>
@@ -3789,7 +3798,7 @@
     </row>
     <row r="116" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B116" s="4" t="s">
         <v>8</v>
@@ -3805,7 +3814,7 @@
     </row>
     <row r="117" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B117" s="4" t="s">
         <v>8</v>
@@ -3821,7 +3830,7 @@
     </row>
     <row r="118" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B118" s="4" t="s">
         <v>8</v>
@@ -3837,7 +3846,7 @@
     </row>
     <row r="119" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B119" s="4" t="s">
         <v>8</v>
@@ -3853,7 +3862,7 @@
     </row>
     <row r="120" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>8</v>
@@ -3868,7 +3877,7 @@
     </row>
     <row r="121" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B121" s="4" t="s">
         <v>8</v>
@@ -3883,7 +3892,7 @@
     </row>
     <row r="122" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B122" s="4" t="s">
         <v>8</v>
@@ -3898,7 +3907,7 @@
     </row>
     <row r="123" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B123" s="4" t="s">
         <v>8</v>
@@ -3913,7 +3922,7 @@
     </row>
     <row r="124" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B124" s="4" t="s">
         <v>8</v>
@@ -3929,7 +3938,7 @@
     </row>
     <row r="125" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B125" s="4" t="s">
         <v>8</v>
@@ -3945,7 +3954,7 @@
     </row>
     <row r="126" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B126" s="4" t="s">
         <v>8</v>
@@ -3960,7 +3969,7 @@
     </row>
     <row r="127" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="6" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B127" s="4" t="s">
         <v>8</v>
@@ -3975,7 +3984,7 @@
     </row>
     <row r="128" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B128" s="4" t="s">
         <v>8</v>
@@ -3990,18 +3999,74 @@
     </row>
     <row r="129" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
+        <v>533</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C129" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D129" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F129" s="1"/>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>534</v>
       </c>
-      <c r="B129" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C129" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D129" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F129" s="1"/>
+      <c r="B130" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C130" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D130" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>535</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C131" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D131" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>536</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C132" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D132" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>537</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C133" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D133" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4132,19 +4197,23 @@
     <hyperlink ref="B127" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
     <hyperlink ref="B128" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
     <hyperlink ref="B129" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="B130" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="B131" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="B132" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="B133" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId128"/>
+  <pageSetup orientation="portrait" r:id="rId132"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AD97"/>
+  <dimension ref="A1:AD101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H94" sqref="H94"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4530,7 +4599,7 @@
         <v>29</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>105</v>
@@ -4598,7 +4667,7 @@
         <v>29</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>105</v>
@@ -4717,7 +4786,7 @@
         <v>29</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>105</v>
@@ -6860,7 +6929,7 @@
     </row>
     <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>28</v>
@@ -6869,7 +6938,7 @@
         <v>29</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="I65" s="2" t="s">
         <v>46</v>
@@ -6908,10 +6977,10 @@
         <v>34</v>
       </c>
       <c r="U65" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="V65" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="W65" s="6"/>
       <c r="X65" s="7" t="s">
@@ -6926,7 +6995,7 @@
     </row>
     <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>28</v>
@@ -6935,7 +7004,7 @@
         <v>29</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="I66" s="2" t="s">
         <v>46</v>
@@ -6974,7 +7043,7 @@
         <v>34</v>
       </c>
       <c r="U66" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="V66" s="6"/>
       <c r="W66" s="6"/>
@@ -6990,7 +7059,7 @@
     </row>
     <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>28</v>
@@ -6999,7 +7068,7 @@
         <v>29</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="I67" s="2" t="s">
         <v>46</v>
@@ -7038,10 +7107,10 @@
         <v>34</v>
       </c>
       <c r="U67" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="V67" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="W67" s="6"/>
       <c r="X67" s="7" t="s">
@@ -7056,7 +7125,7 @@
     </row>
     <row r="68" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>28</v>
@@ -7065,7 +7134,7 @@
         <v>29</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I68" s="2" t="s">
         <v>46</v>
@@ -7089,7 +7158,7 @@
         <v>357</v>
       </c>
       <c r="P68" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="Q68" s="2" t="s">
         <v>358</v>
@@ -7104,10 +7173,10 @@
         <v>34</v>
       </c>
       <c r="U68" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="V68" s="2" t="s">
         <v>483</v>
-      </c>
-      <c r="V68" s="2" t="s">
-        <v>484</v>
       </c>
       <c r="W68" s="6"/>
       <c r="X68" s="7" t="s">
@@ -7122,7 +7191,7 @@
     </row>
     <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>28</v>
@@ -7131,7 +7200,7 @@
         <v>29</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I69" s="2" t="s">
         <v>46</v>
@@ -7155,7 +7224,7 @@
         <v>357</v>
       </c>
       <c r="P69" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="Q69" s="2" t="s">
         <v>358</v>
@@ -7185,7 +7254,7 @@
     </row>
     <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>28</v>
@@ -7194,7 +7263,7 @@
         <v>29</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I70" s="2" t="s">
         <v>46</v>
@@ -7218,7 +7287,7 @@
         <v>357</v>
       </c>
       <c r="P70" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="Q70" s="2" t="s">
         <v>358</v>
@@ -7247,7 +7316,7 @@
     </row>
     <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>28</v>
@@ -7256,7 +7325,7 @@
         <v>29</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I71" s="2" t="s">
         <v>46</v>
@@ -7280,7 +7349,7 @@
         <v>357</v>
       </c>
       <c r="P71" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="Q71" s="2" t="s">
         <v>358</v>
@@ -7295,7 +7364,7 @@
         <v>34</v>
       </c>
       <c r="U71" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="V71" s="2"/>
       <c r="W71" s="6"/>
@@ -7311,7 +7380,7 @@
     </row>
     <row r="72" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>28</v>
@@ -7320,7 +7389,7 @@
         <v>29</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I72" s="2" t="s">
         <v>46</v>
@@ -7344,7 +7413,7 @@
         <v>357</v>
       </c>
       <c r="P72" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="Q72" s="2" t="s">
         <v>358</v>
@@ -7359,7 +7428,7 @@
         <v>34</v>
       </c>
       <c r="U72" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="V72" s="2"/>
       <c r="W72" s="6"/>
@@ -7375,7 +7444,7 @@
     </row>
     <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>28</v>
@@ -7384,7 +7453,7 @@
         <v>29</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="I73" s="2" t="s">
         <v>46</v>
@@ -7408,7 +7477,7 @@
         <v>357</v>
       </c>
       <c r="P73" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="Q73" s="2" t="s">
         <v>358</v>
@@ -7423,7 +7492,7 @@
         <v>34</v>
       </c>
       <c r="U73" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="V73" s="2"/>
       <c r="W73" s="6"/>
@@ -7439,7 +7508,7 @@
     </row>
     <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>28</v>
@@ -7448,7 +7517,7 @@
         <v>29</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="I74" s="2" t="s">
         <v>46</v>
@@ -7472,7 +7541,7 @@
         <v>357</v>
       </c>
       <c r="P74" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="Q74" s="2" t="s">
         <v>358</v>
@@ -7487,7 +7556,7 @@
         <v>34</v>
       </c>
       <c r="U74" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="V74" s="2"/>
       <c r="W74" s="6"/>
@@ -7503,7 +7572,7 @@
     </row>
     <row r="75" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>28</v>
@@ -7512,7 +7581,7 @@
         <v>29</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="I75" s="2" t="s">
         <v>46</v>
@@ -7536,7 +7605,7 @@
         <v>357</v>
       </c>
       <c r="P75" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="Q75" s="2" t="s">
         <v>358</v>
@@ -7551,7 +7620,7 @@
         <v>34</v>
       </c>
       <c r="U75" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="V75" s="2"/>
       <c r="W75" s="6"/>
@@ -7567,7 +7636,7 @@
     </row>
     <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>28</v>
@@ -7576,7 +7645,7 @@
         <v>29</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I76" s="2" t="s">
         <v>46</v>
@@ -7600,7 +7669,7 @@
         <v>357</v>
       </c>
       <c r="P76" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="Q76" s="2" t="s">
         <v>358</v>
@@ -7615,7 +7684,7 @@
         <v>34</v>
       </c>
       <c r="U76" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="V76" s="2"/>
       <c r="W76" s="6"/>
@@ -7631,7 +7700,7 @@
     </row>
     <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>28</v>
@@ -7640,7 +7709,7 @@
         <v>29</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I77" s="2" t="s">
         <v>46</v>
@@ -7664,7 +7733,7 @@
         <v>357</v>
       </c>
       <c r="P77" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="Q77" s="2" t="s">
         <v>358</v>
@@ -7679,7 +7748,7 @@
         <v>34</v>
       </c>
       <c r="U77" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="V77" s="2"/>
       <c r="W77" s="6"/>
@@ -7695,7 +7764,7 @@
     </row>
     <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>28</v>
@@ -7704,7 +7773,7 @@
         <v>29</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I78" s="2" t="s">
         <v>46</v>
@@ -7728,7 +7797,7 @@
         <v>357</v>
       </c>
       <c r="P78" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="Q78" s="2" t="s">
         <v>358</v>
@@ -7743,7 +7812,7 @@
         <v>34</v>
       </c>
       <c r="U78" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="V78" s="2"/>
       <c r="W78" s="6"/>
@@ -7759,7 +7828,7 @@
     </row>
     <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>28</v>
@@ -7768,7 +7837,7 @@
         <v>29</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="I79" s="2" t="s">
         <v>46</v>
@@ -7792,7 +7861,7 @@
         <v>357</v>
       </c>
       <c r="P79" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="Q79" s="2" t="s">
         <v>358</v>
@@ -7807,7 +7876,7 @@
         <v>34</v>
       </c>
       <c r="U79" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="V79" s="2"/>
       <c r="W79" s="6"/>
@@ -7823,7 +7892,7 @@
     </row>
     <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>28</v>
@@ -7832,7 +7901,7 @@
         <v>29</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="I80" s="2" t="s">
         <v>46</v>
@@ -7856,7 +7925,7 @@
         <v>357</v>
       </c>
       <c r="P80" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="Q80" s="2" t="s">
         <v>358</v>
@@ -7871,7 +7940,7 @@
         <v>34</v>
       </c>
       <c r="U80" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="V80" s="2"/>
       <c r="W80" s="6"/>
@@ -7887,7 +7956,7 @@
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>28</v>
@@ -7896,7 +7965,7 @@
         <v>29</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I81" s="2" t="s">
         <v>46</v>
@@ -7920,7 +7989,7 @@
         <v>357</v>
       </c>
       <c r="P81" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="Q81" s="2" t="s">
         <v>358</v>
@@ -7935,7 +8004,7 @@
         <v>34</v>
       </c>
       <c r="U81" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="V81" s="2"/>
       <c r="W81" s="6"/>
@@ -7951,7 +8020,7 @@
     </row>
     <row r="82" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>28</v>
@@ -7960,10 +8029,10 @@
         <v>29</v>
       </c>
       <c r="H82" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="I82" s="2" t="s">
         <v>524</v>
-      </c>
-      <c r="I82" s="2" t="s">
-        <v>525</v>
       </c>
       <c r="J82" s="6" t="s">
         <v>35</v>
@@ -8010,7 +8079,7 @@
     </row>
     <row r="83" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>28</v>
@@ -8019,10 +8088,10 @@
         <v>29</v>
       </c>
       <c r="H83" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="I83" s="2" t="s">
         <v>524</v>
-      </c>
-      <c r="I83" s="2" t="s">
-        <v>525</v>
       </c>
       <c r="J83" s="6" t="s">
         <v>35</v>
@@ -8069,7 +8138,7 @@
     </row>
     <row r="84" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>28</v>
@@ -8078,10 +8147,10 @@
         <v>29</v>
       </c>
       <c r="H84" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="I84" s="2" t="s">
         <v>524</v>
-      </c>
-      <c r="I84" s="2" t="s">
-        <v>525</v>
       </c>
       <c r="J84" s="6" t="s">
         <v>35</v>
@@ -8128,7 +8197,7 @@
     </row>
     <row r="85" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>28</v>
@@ -8137,10 +8206,10 @@
         <v>29</v>
       </c>
       <c r="H85" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="I85" s="2" t="s">
         <v>524</v>
-      </c>
-      <c r="I85" s="2" t="s">
-        <v>525</v>
       </c>
       <c r="J85" s="6" t="s">
         <v>35</v>
@@ -8187,7 +8256,7 @@
     </row>
     <row r="86" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>28</v>
@@ -8196,10 +8265,10 @@
         <v>29</v>
       </c>
       <c r="H86" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="I86" s="2" t="s">
         <v>524</v>
-      </c>
-      <c r="I86" s="2" t="s">
-        <v>525</v>
       </c>
       <c r="J86" s="6" t="s">
         <v>35</v>
@@ -8246,7 +8315,7 @@
     </row>
     <row r="87" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>28</v>
@@ -8255,10 +8324,10 @@
         <v>29</v>
       </c>
       <c r="H87" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="I87" s="2" t="s">
         <v>524</v>
-      </c>
-      <c r="I87" s="2" t="s">
-        <v>525</v>
       </c>
       <c r="J87" s="6" t="s">
         <v>35</v>
@@ -8305,7 +8374,7 @@
     </row>
     <row r="88" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>28</v>
@@ -8314,10 +8383,10 @@
         <v>29</v>
       </c>
       <c r="H88" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="I88" s="2" t="s">
         <v>524</v>
-      </c>
-      <c r="I88" s="2" t="s">
-        <v>525</v>
       </c>
       <c r="J88" s="6" t="s">
         <v>35</v>
@@ -8364,7 +8433,7 @@
     </row>
     <row r="89" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>28</v>
@@ -8373,10 +8442,10 @@
         <v>29</v>
       </c>
       <c r="H89" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="I89" s="2" t="s">
         <v>524</v>
-      </c>
-      <c r="I89" s="2" t="s">
-        <v>525</v>
       </c>
       <c r="J89" s="6" t="s">
         <v>35</v>
@@ -8423,7 +8492,7 @@
     </row>
     <row r="90" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>28</v>
@@ -8432,10 +8501,10 @@
         <v>29</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="J90" s="6" t="s">
         <v>35</v>
@@ -8482,7 +8551,7 @@
     </row>
     <row r="91" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>28</v>
@@ -8491,10 +8560,10 @@
         <v>29</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="J91" s="6" t="s">
         <v>35</v>
@@ -8541,7 +8610,7 @@
     </row>
     <row r="92" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="F92" s="2" t="s">
         <v>28</v>
@@ -8550,10 +8619,10 @@
         <v>29</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="J92" s="6" t="s">
         <v>35</v>
@@ -8600,7 +8669,7 @@
     </row>
     <row r="93" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>28</v>
@@ -8609,10 +8678,10 @@
         <v>29</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="J93" s="6" t="s">
         <v>35</v>
@@ -8659,7 +8728,7 @@
     </row>
     <row r="94" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>28</v>
@@ -8668,10 +8737,10 @@
         <v>29</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>535</v>
+        <v>526</v>
       </c>
       <c r="I94" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="J94" s="6" t="s">
         <v>35</v>
@@ -8718,7 +8787,7 @@
     </row>
     <row r="95" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>28</v>
@@ -8727,10 +8796,10 @@
         <v>29</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="J95" s="6" t="s">
         <v>35</v>
@@ -8777,7 +8846,7 @@
     </row>
     <row r="96" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>28</v>
@@ -8786,10 +8855,10 @@
         <v>29</v>
       </c>
       <c r="H96" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="I96" s="2" t="s">
         <v>524</v>
-      </c>
-      <c r="I96" s="2" t="s">
-        <v>525</v>
       </c>
       <c r="J96" s="6" t="s">
         <v>35</v>
@@ -8836,7 +8905,7 @@
     </row>
     <row r="97" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>28</v>
@@ -8845,10 +8914,10 @@
         <v>29</v>
       </c>
       <c r="H97" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="I97" s="2" t="s">
         <v>524</v>
-      </c>
-      <c r="I97" s="2" t="s">
-        <v>525</v>
       </c>
       <c r="J97" s="6" t="s">
         <v>35</v>
@@ -8890,6 +8959,242 @@
         <v>85</v>
       </c>
       <c r="Z97" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="98" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="6" t="s">
+        <v>534</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="I98" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="J98" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K98" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L98" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M98" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N98" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O98" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P98" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q98" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R98" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S98" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T98" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X98" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y98" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z98" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="99" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="I99" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="J99" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K99" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L99" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M99" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N99" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O99" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P99" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q99" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R99" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S99" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T99" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X99" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y99" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z99" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="100" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="I100" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="J100" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K100" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L100" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M100" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N100" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O100" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P100" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q100" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R100" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S100" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T100" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X100" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y100" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z100" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="101" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="6" t="s">
+        <v>537</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H101" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="I101" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="J101" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K101" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L101" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M101" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N101" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O101" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P101" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q101" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R101" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S101" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T101" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X101" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y101" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z101" s="7" t="s">
         <v>82</v>
       </c>
     </row>
@@ -8982,7 +9287,7 @@
   <dimension ref="A1:AM21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10090,7 +10395,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AE11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10306,7 +10613,7 @@
         <v>29</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>431</v>
+        <v>538</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>403</v>
@@ -10445,7 +10752,7 @@
         <v>29</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>422</v>
@@ -10498,7 +10805,7 @@
         <v>29</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>426</v>
@@ -10542,13 +10849,13 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>444</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>445</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>446</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>28</v>
@@ -10557,10 +10864,10 @@
         <v>29</v>
       </c>
       <c r="F7" s="11" t="s">
+        <v>446</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>447</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>448</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>35</v>
@@ -10593,15 +10900,15 @@
         <v>391</v>
       </c>
       <c r="R7" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="S7" s="9" t="s">
         <v>449</v>
-      </c>
-      <c r="S7" s="9" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B8" s="6">
         <v>500</v>
@@ -10616,10 +10923,10 @@
         <v>29</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>35</v>
@@ -10652,45 +10959,45 @@
         <v>391</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="S8" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="T8" s="9" t="s">
         <v>104</v>
       </c>
       <c r="U8" s="9" t="s">
+        <v>453</v>
+      </c>
+      <c r="V8" s="9" t="s">
         <v>454</v>
       </c>
-      <c r="V8" s="9" t="s">
+      <c r="W8" s="9" t="s">
         <v>455</v>
       </c>
-      <c r="W8" s="9" t="s">
+      <c r="X8" s="9" t="s">
         <v>456</v>
       </c>
-      <c r="X8" s="9" t="s">
+      <c r="Y8" s="6" t="s">
         <v>457</v>
-      </c>
-      <c r="Y8" s="6" t="s">
-        <v>458</v>
       </c>
       <c r="Z8" s="9" t="s">
         <v>211</v>
       </c>
       <c r="AA8" s="9" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>464</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>465</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>28</v>
@@ -10699,10 +11006,10 @@
         <v>29</v>
       </c>
       <c r="F9" s="11" t="s">
+        <v>461</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>462</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>463</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>35</v>
@@ -10735,21 +11042,21 @@
         <v>391</v>
       </c>
       <c r="R9" s="6" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="S9" s="9" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>473</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>474</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>28</v>
@@ -10758,10 +11065,10 @@
         <v>29</v>
       </c>
       <c r="F10" s="11" t="s">
+        <v>469</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>470</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>471</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>35</v>
@@ -10794,21 +11101,21 @@
         <v>391</v>
       </c>
       <c r="R10" s="6" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="S10" s="9" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>480</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>481</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>28</v>
@@ -10817,10 +11124,10 @@
         <v>29</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>35</v>
@@ -10853,22 +11160,22 @@
         <v>391</v>
       </c>
       <c r="R11" s="6" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="S11" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="T11" s="9" t="s">
         <v>104</v>
       </c>
       <c r="U11" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="V11" s="6">
         <v>1000</v>
       </c>
       <c r="W11" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>